<commit_message>
update table from cruise to month
</commit_message>
<xml_diff>
--- a/table/BCc/biomass_BCD.xlsx
+++ b/table/BCc/biomass_BCD.xlsx
@@ -389,16 +389,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.8509092159840681</v>
+        <v>0.8509092159840699</v>
       </c>
       <c r="C2">
-        <v>0.0003564971602369188</v>
+        <v>0.0003564971602369523</v>
       </c>
       <c r="D2">
-        <v>0.7806962301593611</v>
+        <v>0.7806962301593607</v>
       </c>
       <c r="E2">
-        <v>1.412204170184479e-005</v>
+        <v>1.412204170184457e-05</v>
       </c>
     </row>
     <row r="3">
@@ -406,16 +406,16 @@
         <v>0.1</v>
       </c>
       <c r="B3">
-        <v>0.8734789077030982</v>
+        <v>0.8734789077030988</v>
       </c>
       <c r="C3">
-        <v>0.001170690556095257</v>
+        <v>0.001170690556095291</v>
       </c>
       <c r="D3">
-        <v>0.945960111102199</v>
+        <v>0.9459601111021961</v>
       </c>
       <c r="E3">
-        <v>0.1013746584607922</v>
+        <v>0.1013746584607724</v>
       </c>
     </row>
     <row r="4">
@@ -426,13 +426,13 @@
         <v>0.8656969518537667</v>
       </c>
       <c r="C4">
-        <v>0.0007693835755932071</v>
+        <v>0.0007693835755932047</v>
       </c>
       <c r="D4">
-        <v>0.8849651696460288</v>
+        <v>0.8849651696460281</v>
       </c>
       <c r="E4">
-        <v>0.002219412612370729</v>
+        <v>0.002219412612370646</v>
       </c>
     </row>
     <row r="5">
@@ -440,16 +440,16 @@
         <v>0.25</v>
       </c>
       <c r="B5">
-        <v>0.8408742198261066</v>
+        <v>0.8408742198261075</v>
       </c>
       <c r="C5">
-        <v>0.0002157584515181243</v>
+        <v>0.000215758451518134</v>
       </c>
       <c r="D5">
-        <v>0.8528955196665423</v>
+        <v>0.8528955196665418</v>
       </c>
       <c r="E5">
-        <v>0.0003944839033909362</v>
+        <v>0.0003944839033909248</v>
       </c>
     </row>
     <row r="6">
@@ -457,16 +457,16 @@
         <v>0.3</v>
       </c>
       <c r="B6">
-        <v>0.833953879044985</v>
+        <v>0.833953879044983</v>
       </c>
       <c r="C6">
-        <v>0.0001539494423392302</v>
+        <v>0.0001539494423392158</v>
       </c>
       <c r="D6">
-        <v>0.8270150827740983</v>
+        <v>0.8270150827740971</v>
       </c>
       <c r="E6">
-        <v>0.0001105021877597798</v>
+        <v>0.0001105021877597733</v>
       </c>
     </row>
     <row r="7">
@@ -474,16 +474,16 @@
         <v>0.4</v>
       </c>
       <c r="B7">
-        <v>0.8397327879019978</v>
+        <v>0.8397327879019963</v>
       </c>
       <c r="C7">
-        <v>0.0002039765540052356</v>
+        <v>0.0002039765540052206</v>
       </c>
       <c r="D7">
-        <v>0.7994153328468536</v>
+        <v>0.7994153328468506</v>
       </c>
       <c r="E7">
-        <v>3.145685980735156e-005</v>
+        <v>3.145685980734743e-05</v>
       </c>
     </row>
     <row r="8">
@@ -491,16 +491,16 @@
         <v>0.5</v>
       </c>
       <c r="B8">
-        <v>0.839944461853305</v>
+        <v>0.8399444618533058</v>
       </c>
       <c r="C8">
-        <v>0.0002061087867805871</v>
+        <v>0.0002061087867805954</v>
       </c>
       <c r="D8">
-        <v>0.7583763256917896</v>
+        <v>0.758376325691787</v>
       </c>
       <c r="E8">
-        <v>5.699558704515901e-006</v>
+        <v>5.699558704515319e-06</v>
       </c>
     </row>
     <row r="9">
@@ -508,16 +508,16 @@
         <v>0.6</v>
       </c>
       <c r="B9">
-        <v>0.8416012743436624</v>
+        <v>0.8416012743436532</v>
       </c>
       <c r="C9">
-        <v>0.0002236380315347403</v>
+        <v>0.0002236380315346383</v>
       </c>
       <c r="D9">
-        <v>0.7283313129323578</v>
+        <v>0.7283313129323612</v>
       </c>
       <c r="E9">
-        <v>1.805985571180473e-006</v>
+        <v>1.805985571180705e-06</v>
       </c>
     </row>
     <row r="10">
@@ -525,16 +525,16 @@
         <v>0.7</v>
       </c>
       <c r="B10">
-        <v>0.8431823265072063</v>
+        <v>0.8431823265071985</v>
       </c>
       <c r="C10">
-        <v>0.0002418464009775519</v>
+        <v>0.0002418464009774582</v>
       </c>
       <c r="D10">
-        <v>0.7125975310765524</v>
+        <v>0.7125975310765174</v>
       </c>
       <c r="E10">
-        <v>1.018866505713978e-006</v>
+        <v>1.018866505712703e-06</v>
       </c>
     </row>
     <row r="11">
@@ -542,16 +542,16 @@
         <v>0.8</v>
       </c>
       <c r="B11">
-        <v>0.8535066042050612</v>
+        <v>0.8535066042050603</v>
       </c>
       <c r="C11">
-        <v>0.0004070169720084024</v>
+        <v>0.0004070169720083852</v>
       </c>
       <c r="D11">
-        <v>0.6938683632830103</v>
+        <v>0.6938683632829428</v>
       </c>
       <c r="E11">
-        <v>5.278673829037693e-007</v>
+        <v>5.278673829025448e-07</v>
       </c>
     </row>
     <row r="12">
@@ -559,16 +559,16 @@
         <v>0.9</v>
       </c>
       <c r="B12">
-        <v>0.8461045448792828</v>
+        <v>0.8461045448792888</v>
       </c>
       <c r="C12">
-        <v>0.0002797701294392631</v>
+        <v>0.0002797701294393467</v>
       </c>
       <c r="D12">
-        <v>0.6766217350143513</v>
+        <v>0.6766217350145254</v>
       </c>
       <c r="E12">
-        <v>2.942546768325853e-007</v>
+        <v>2.942546768342929e-07</v>
       </c>
     </row>
     <row r="13">
@@ -576,16 +576,16 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>0.8290633937894685</v>
+        <v>0.8290633937894669</v>
       </c>
       <c r="C13">
-        <v>0.0001217808445520538</v>
+        <v>0.0001217808445520448</v>
       </c>
       <c r="D13">
-        <v>0.6625136387329526</v>
+        <v>0.6625136387332591</v>
       </c>
       <c r="E13">
-        <v>1.850100096270231e-007</v>
+        <v>1.850100096288642e-07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>